<commit_message>
Added entry for 1st position in Chakravyuh CTF, organized by LPU SCSE.
</commit_message>
<xml_diff>
--- a/training_certs_record.xlsx
+++ b/training_certs_record.xlsx
@@ -16,7 +16,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="249">
+  <si>
+    <t xml:space="preserve">1st Position - Chakravyuh CTF - 12 Hours CTF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L.P.U. School of Computer Science and Engineering</t>
+  </si>
   <si>
     <t xml:space="preserve">Introduction to Hacking Methodology</t>
   </si>
@@ -814,10 +820,10 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="17" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="17" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="17" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1336,7 +1342,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="100" workbookViewId="0">
       <selection activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1358,119 +1364,119 @@
         <v>1</v>
       </c>
       <c r="C1" s="3">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4">
         <v>45689</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="5">
-        <v>45627</v>
-      </c>
-      <c r="D2" s="1">
-        <v>127699968</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="4">
+        <v>45627</v>
+      </c>
+      <c r="D3" s="1">
+        <v>127699968</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -1478,134 +1484,134 @@
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="4" t="s">
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" ht="42.75">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="E12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1" t="s">
+    </row>
+    <row r="13" ht="42.75">
+      <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="E13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="1" t="s">
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" ht="28.5">
-      <c r="A14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="E14" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="1">
-        <v>8835432</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" ht="28.5">
       <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1">
-        <v>8835521</v>
-      </c>
-      <c r="E15" s="4" t="s">
+        <v>8835432</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="28.5">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1">
+        <v>8835521</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19">
@@ -1615,8 +1621,8 @@
       <c r="B19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>48</v>
+      <c r="C19" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20">
@@ -1626,100 +1632,97 @@
       <c r="B20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>57</v>
+      <c r="C20" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="E21" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="E25" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="1">
-        <v>100019282</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="D26" s="1">
+        <v>100019282</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1728,156 +1731,156 @@
         <v>76</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="E28" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="E29" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="E30" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="1" t="s">
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="B32" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="32" ht="27">
-      <c r="A32" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="E32" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E32" s="7" t="s">
+    </row>
+    <row r="33" ht="27">
+      <c r="A33" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="s">
+      <c r="B33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="E33" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="E34" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="5" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1886,283 +1889,283 @@
         <v>112</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="D37" s="1">
-        <v>908449736</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="D38" s="1">
+        <v>908449736</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="E39" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="E41" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C41" s="1" t="s">
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="C42" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="42" ht="28.5">
-      <c r="A42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="E42" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="43" ht="28.5">
       <c r="A43" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="44" ht="28.5">
       <c r="A44" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="E44" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C44" s="1" t="s">
+    </row>
+    <row r="45" ht="28.5">
+      <c r="A45" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="C45" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="E45" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C45" s="1" t="s">
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D45" s="1">
+      <c r="B46" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="1">
         <v>1246352</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="46" ht="28.5">
-      <c r="A46" s="1" t="s">
+      <c r="E46" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" ht="28.5">
+      <c r="A47" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1246352</v>
+      <c r="E47" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>156</v>
+        <v>148</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1246352</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="E49" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1246352</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="D50" s="1">
+        <v>1246352</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="C51" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D51" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="E52" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D53" s="1">
-        <v>2350911</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="C54" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D54" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" s="1">
+        <v>2350911</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2171,91 +2174,94 @@
         <v>175</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="C56" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D56" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="E57" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="E59" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="E60" s="5" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2264,12 +2270,9 @@
         <v>194</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>176</v>
+        <v>52</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E61" s="4" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2278,35 +2281,38 @@
         <v>196</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D63" s="1" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="65">
@@ -2317,45 +2323,42 @@
         <v>204</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="C66" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E68" s="4" t="s">
+      <c r="E68" s="5" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2364,9 +2367,12 @@
         <v>212</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>202</v>
+        <v>125</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2375,60 +2381,54 @@
         <v>214</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="E72" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D72" s="1">
-        <v>46292805</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="D73" s="1">
-        <v>46873384</v>
-      </c>
-      <c r="E73" s="4" t="s">
+        <v>46292805</v>
+      </c>
+      <c r="E73" s="5" t="s">
         <v>224</v>
       </c>
     </row>
@@ -2437,50 +2437,50 @@
         <v>225</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>176</v>
+        <v>222</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D74" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D74" s="1">
+        <v>46873384</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>226</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D75" s="1" t="s">
+      <c r="E75" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D76" s="1" t="s">
+      <c r="E76" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="77">
@@ -2488,16 +2488,16 @@
         <v>233</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E77" s="4" t="s">
-        <v>230</v>
+      <c r="E77" s="5" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="78">
@@ -2505,114 +2505,131 @@
         <v>235</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>238</v>
+      <c r="E78" s="5" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="E79" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="E80" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D80" s="1" t="s">
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="B81" s="1" t="s">
         <v>246</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E1"/>
-    <hyperlink r:id="rId2" ref="E2"/>
-    <hyperlink r:id="rId3" ref="E6"/>
-    <hyperlink r:id="rId4" ref="E7"/>
-    <hyperlink r:id="rId5" ref="E8"/>
-    <hyperlink r:id="rId6" ref="E10"/>
-    <hyperlink r:id="rId7" ref="E11"/>
-    <hyperlink r:id="rId8" ref="E12"/>
-    <hyperlink r:id="rId9" ref="E13"/>
-    <hyperlink r:id="rId10" ref="E14"/>
-    <hyperlink r:id="rId11" ref="E15"/>
-    <hyperlink r:id="rId12" ref="E20"/>
-    <hyperlink r:id="rId13" ref="E21"/>
-    <hyperlink r:id="rId14" ref="E22"/>
-    <hyperlink r:id="rId15" ref="E23"/>
-    <hyperlink r:id="rId16" ref="E24"/>
-    <hyperlink r:id="rId17" ref="E25"/>
-    <hyperlink r:id="rId18" ref="E26"/>
-    <hyperlink r:id="rId19" ref="E27"/>
-    <hyperlink r:id="rId20" ref="E28"/>
-    <hyperlink r:id="rId21" ref="E29"/>
-    <hyperlink r:id="rId22" ref="E31"/>
-    <hyperlink r:id="rId23" ref="D32"/>
-    <hyperlink r:id="rId24" ref="E32"/>
-    <hyperlink r:id="rId25" ref="E33"/>
-    <hyperlink r:id="rId26" ref="E34"/>
-    <hyperlink r:id="rId27" ref="E35"/>
-    <hyperlink r:id="rId28" ref="E36"/>
-    <hyperlink r:id="rId29" ref="E37"/>
-    <hyperlink r:id="rId30" ref="E38"/>
-    <hyperlink r:id="rId31" ref="E40"/>
-    <hyperlink r:id="rId32" ref="E41"/>
-    <hyperlink r:id="rId33" ref="E42"/>
-    <hyperlink r:id="rId34" ref="E43"/>
-    <hyperlink r:id="rId35" ref="E44"/>
-    <hyperlink r:id="rId36" ref="E45"/>
-    <hyperlink r:id="rId37" ref="E46"/>
-    <hyperlink r:id="rId38" ref="E48"/>
-    <hyperlink r:id="rId39" ref="E49"/>
-    <hyperlink r:id="rId40" ref="E51"/>
-    <hyperlink r:id="rId41" ref="E53"/>
-    <hyperlink r:id="rId42" ref="E55"/>
-    <hyperlink r:id="rId43" ref="E56"/>
-    <hyperlink r:id="rId44" ref="E57"/>
-    <hyperlink r:id="rId45" ref="E58"/>
-    <hyperlink r:id="rId46" ref="E59"/>
-    <hyperlink r:id="rId47" ref="E61"/>
-    <hyperlink r:id="rId48" ref="E65"/>
-    <hyperlink r:id="rId49" ref="E67"/>
-    <hyperlink r:id="rId50" ref="E68"/>
-    <hyperlink r:id="rId51" ref="E71"/>
-    <hyperlink r:id="rId52" ref="E72"/>
-    <hyperlink r:id="rId53" ref="E73"/>
-    <hyperlink r:id="rId54" ref="E74"/>
-    <hyperlink r:id="rId55" ref="E75"/>
+    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink r:id="rId2" ref="E3"/>
+    <hyperlink r:id="rId3" ref="E7"/>
+    <hyperlink r:id="rId4" ref="E8"/>
+    <hyperlink r:id="rId5" ref="E9"/>
+    <hyperlink r:id="rId6" ref="E11"/>
+    <hyperlink r:id="rId7" ref="E12"/>
+    <hyperlink r:id="rId8" ref="E13"/>
+    <hyperlink r:id="rId9" ref="E14"/>
+    <hyperlink r:id="rId10" ref="E15"/>
+    <hyperlink r:id="rId11" ref="E16"/>
+    <hyperlink r:id="rId12" ref="E21"/>
+    <hyperlink r:id="rId13" ref="E22"/>
+    <hyperlink r:id="rId14" ref="E23"/>
+    <hyperlink r:id="rId15" ref="E24"/>
+    <hyperlink r:id="rId16" ref="E25"/>
+    <hyperlink r:id="rId17" ref="E26"/>
+    <hyperlink r:id="rId18" ref="E27"/>
+    <hyperlink r:id="rId19" ref="E28"/>
+    <hyperlink r:id="rId20" ref="E29"/>
+    <hyperlink r:id="rId21" ref="E30"/>
+    <hyperlink r:id="rId22" ref="E32"/>
+    <hyperlink r:id="rId23" ref="D33"/>
+    <hyperlink r:id="rId24" ref="E33"/>
+    <hyperlink r:id="rId25" ref="E34"/>
+    <hyperlink r:id="rId26" ref="E35"/>
+    <hyperlink r:id="rId27" ref="E36"/>
+    <hyperlink r:id="rId28" ref="E37"/>
+    <hyperlink r:id="rId29" ref="E38"/>
+    <hyperlink r:id="rId30" ref="E39"/>
+    <hyperlink r:id="rId31" ref="E41"/>
+    <hyperlink r:id="rId32" ref="E42"/>
+    <hyperlink r:id="rId33" ref="E43"/>
+    <hyperlink r:id="rId34" ref="E44"/>
+    <hyperlink r:id="rId35" ref="E45"/>
+    <hyperlink r:id="rId36" ref="E46"/>
+    <hyperlink r:id="rId37" ref="E47"/>
+    <hyperlink r:id="rId38" ref="E49"/>
+    <hyperlink r:id="rId39" ref="E50"/>
+    <hyperlink r:id="rId40" ref="E52"/>
+    <hyperlink r:id="rId41" ref="E54"/>
+    <hyperlink r:id="rId42" ref="E56"/>
+    <hyperlink r:id="rId43" ref="E57"/>
+    <hyperlink r:id="rId44" ref="E58"/>
+    <hyperlink r:id="rId45" ref="E59"/>
+    <hyperlink r:id="rId46" ref="E60"/>
+    <hyperlink r:id="rId47" ref="E62"/>
+    <hyperlink r:id="rId48" ref="E66"/>
+    <hyperlink r:id="rId49" ref="E68"/>
+    <hyperlink r:id="rId50" ref="E69"/>
+    <hyperlink r:id="rId51" ref="E72"/>
+    <hyperlink r:id="rId52" ref="E73"/>
+    <hyperlink r:id="rId53" ref="E74"/>
+    <hyperlink r:id="rId54" ref="E75"/>
     <hyperlink r:id="rId55" ref="E76"/>
     <hyperlink r:id="rId55" ref="E77"/>
-    <hyperlink r:id="rId56" ref="E78"/>
-    <hyperlink r:id="rId57" ref="E79"/>
-    <hyperlink r:id="rId58" ref="E80"/>
+    <hyperlink r:id="rId55" ref="E78"/>
+    <hyperlink r:id="rId56" ref="E79"/>
+    <hyperlink r:id="rId57" ref="E80"/>
+    <hyperlink r:id="rId58" ref="E81"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Added basic cloud course that I did to be a member of AWS ETC.
</commit_message>
<xml_diff>
--- a/training_certs_record.xlsx
+++ b/training_certs_record.xlsx
@@ -16,7 +16,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="252">
+  <si>
+    <t xml:space="preserve">AWS Educate Introduction to Cloud 101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon Web Services Training and Certification</t>
+  </si>
+  <si>
+    <t>https://www.credly.com/badges/b4a359ff-3f8a-4af8-8f97-4483f500c03d/public_url</t>
+  </si>
   <si>
     <t xml:space="preserve">1st Position - Chakravyuh CTF - 12 Hours CTF</t>
   </si>
@@ -809,21 +818,18 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="17" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="17" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="17" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1357,47 +1363,44 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="2">
         <v>45717</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="4">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4">
         <v>45689</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4">
-        <v>45627</v>
-      </c>
-      <c r="D3" s="1">
-        <v>127699968</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1408,7 +1411,13 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4">
+        <v>45627</v>
+      </c>
+      <c r="D4" s="1">
+        <v>127699968</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1417,65 +1426,59 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1484,27 +1487,27 @@
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
+      <c r="E10" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
@@ -1512,63 +1515,63 @@
         <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" ht="42.75">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="5" t="s">
+    </row>
+    <row r="14" ht="42.75">
+      <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="5" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" ht="28.5">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1">
-        <v>8835432</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1577,29 +1580,32 @@
         <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D16" s="1">
+        <v>8835432</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" ht="28.5">
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="1">
         <v>8835521</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1610,7 +1616,10 @@
       <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1622,54 +1631,51 @@
         <v>52</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>59</v>
+      <c r="C21" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>64</v>
@@ -1677,128 +1683,131 @@
       <c r="D23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="5" t="s">
         <v>68</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="E26" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D26" s="1">
-        <v>100019282</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" s="5" t="s">
         <v>77</v>
+      </c>
+      <c r="D27" s="1">
+        <v>100019282</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="E31" s="3" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1810,60 +1819,57 @@
         <v>95</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="5" t="s">
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="33" ht="27">
-      <c r="A33" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" ht="27">
       <c r="A34" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="E34" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="3" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1872,15 +1878,12 @@
         <v>109</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E36" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1889,29 +1892,29 @@
         <v>112</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E37" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>113</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" s="1">
-        <v>908449736</v>
-      </c>
-      <c r="E38" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1920,26 +1923,32 @@
         <v>117</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="1">
+        <v>908449736</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="E40" s="3" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1950,64 +1959,58 @@
       <c r="B41" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="E42" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D42" s="1" t="s">
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="B43" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="43" ht="28.5">
-      <c r="A43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="44" ht="28.5">
       <c r="A44" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="C44" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="3" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2016,97 +2019,97 @@
         <v>141</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="E45" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D45" s="1" t="s">
+    </row>
+    <row r="46" ht="28.5">
+      <c r="A46" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="B46" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="E46" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D46" s="1">
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D47" s="1">
         <v>1246352</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" ht="28.5">
-      <c r="A47" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="E47" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" ht="28.5">
+      <c r="A48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1246352</v>
+      <c r="D48" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>158</v>
+        <v>151</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1246352</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D50" s="1">
-        <v>1246352</v>
-      </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="3" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2115,9 +2118,15 @@
         <v>162</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1">
+        <v>1246352</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2126,15 +2135,9 @@
         <v>165</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E52" s="5" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2143,29 +2146,29 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="E53" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D54" s="1">
-        <v>2350911</v>
-      </c>
-      <c r="E54" s="5" t="s">
+      <c r="D54" s="1" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2174,26 +2177,29 @@
         <v>175</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
+      </c>
+      <c r="D55" s="1">
+        <v>2350911</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E56" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2202,15 +2208,12 @@
         <v>180</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="3" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2219,32 +2222,32 @@
         <v>183</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="C59" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="E59" s="3" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2253,91 +2256,94 @@
         <v>190</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="C61" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>195</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>178</v>
+        <v>55</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C63" s="1" t="s">
+      <c r="E63" s="3" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>162</v>
+        <v>201</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>201</v>
+      <c r="D65" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67">
@@ -2345,21 +2351,24 @@
         <v>208</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>201</v>
+      <c r="E67" s="3" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>211</v>
+        <v>207</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="69">
@@ -2367,102 +2376,96 @@
         <v>212</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E69" s="5" t="s">
         <v>213</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>215</v>
+      <c r="E70" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="C73" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="E73" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="D73" s="1">
-        <v>46292805</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="C74" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D74" s="1">
-        <v>46873384</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>226</v>
+        <v>46292805</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>178</v>
+        <v>225</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E75" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D75" s="1">
+        <v>46873384</v>
+      </c>
+      <c r="E75" s="3" t="s">
         <v>229</v>
       </c>
     </row>
@@ -2471,15 +2474,15 @@
         <v>230</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="E76" s="3" t="s">
         <v>232</v>
       </c>
     </row>
@@ -2488,100 +2491,117 @@
         <v>233</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E77" s="5" t="s">
-        <v>232</v>
+      <c r="E77" s="3" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>238</v>
+        <v>181</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>115</v>
+        <v>173</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E79" s="5" t="s">
-        <v>240</v>
+      <c r="E79" s="3" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D80" s="1" t="s">
+      <c r="E80" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="C81" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D81" s="1" t="s">
+      <c r="E81" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="E81" s="5" t="s">
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
         <v>248</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink r:id="rId1" ref="E1"/>
     <hyperlink r:id="rId2" ref="E3"/>
-    <hyperlink r:id="rId3" ref="E7"/>
+    <hyperlink r:id="rId3" ref="E4"/>
     <hyperlink r:id="rId4" ref="E8"/>
     <hyperlink r:id="rId5" ref="E9"/>
-    <hyperlink r:id="rId6" ref="E11"/>
+    <hyperlink r:id="rId6" ref="E10"/>
     <hyperlink r:id="rId7" ref="E12"/>
     <hyperlink r:id="rId8" ref="E13"/>
     <hyperlink r:id="rId9" ref="E14"/>
     <hyperlink r:id="rId10" ref="E15"/>
     <hyperlink r:id="rId11" ref="E16"/>
-    <hyperlink r:id="rId12" ref="E21"/>
+    <hyperlink r:id="rId12" ref="E17"/>
     <hyperlink r:id="rId13" ref="E22"/>
     <hyperlink r:id="rId14" ref="E23"/>
     <hyperlink r:id="rId15" ref="E24"/>
@@ -2591,45 +2611,46 @@
     <hyperlink r:id="rId19" ref="E28"/>
     <hyperlink r:id="rId20" ref="E29"/>
     <hyperlink r:id="rId21" ref="E30"/>
-    <hyperlink r:id="rId22" ref="E32"/>
-    <hyperlink r:id="rId23" ref="D33"/>
-    <hyperlink r:id="rId24" ref="E33"/>
+    <hyperlink r:id="rId22" ref="E31"/>
+    <hyperlink r:id="rId23" ref="E33"/>
+    <hyperlink r:id="rId24" ref="D34"/>
     <hyperlink r:id="rId25" ref="E34"/>
     <hyperlink r:id="rId26" ref="E35"/>
     <hyperlink r:id="rId27" ref="E36"/>
     <hyperlink r:id="rId28" ref="E37"/>
     <hyperlink r:id="rId29" ref="E38"/>
     <hyperlink r:id="rId30" ref="E39"/>
-    <hyperlink r:id="rId31" ref="E41"/>
+    <hyperlink r:id="rId31" ref="E40"/>
     <hyperlink r:id="rId32" ref="E42"/>
     <hyperlink r:id="rId33" ref="E43"/>
     <hyperlink r:id="rId34" ref="E44"/>
     <hyperlink r:id="rId35" ref="E45"/>
     <hyperlink r:id="rId36" ref="E46"/>
     <hyperlink r:id="rId37" ref="E47"/>
-    <hyperlink r:id="rId38" ref="E49"/>
+    <hyperlink r:id="rId38" ref="E48"/>
     <hyperlink r:id="rId39" ref="E50"/>
-    <hyperlink r:id="rId40" ref="E52"/>
-    <hyperlink r:id="rId41" ref="E54"/>
-    <hyperlink r:id="rId42" ref="E56"/>
+    <hyperlink r:id="rId40" ref="E51"/>
+    <hyperlink r:id="rId41" ref="E53"/>
+    <hyperlink r:id="rId42" ref="E55"/>
     <hyperlink r:id="rId43" ref="E57"/>
     <hyperlink r:id="rId44" ref="E58"/>
     <hyperlink r:id="rId45" ref="E59"/>
     <hyperlink r:id="rId46" ref="E60"/>
-    <hyperlink r:id="rId47" ref="E62"/>
-    <hyperlink r:id="rId48" ref="E66"/>
-    <hyperlink r:id="rId49" ref="E68"/>
+    <hyperlink r:id="rId47" ref="E61"/>
+    <hyperlink r:id="rId48" ref="E63"/>
+    <hyperlink r:id="rId49" ref="E67"/>
     <hyperlink r:id="rId50" ref="E69"/>
-    <hyperlink r:id="rId51" ref="E72"/>
+    <hyperlink r:id="rId51" ref="E70"/>
     <hyperlink r:id="rId52" ref="E73"/>
     <hyperlink r:id="rId53" ref="E74"/>
     <hyperlink r:id="rId54" ref="E75"/>
     <hyperlink r:id="rId55" ref="E76"/>
-    <hyperlink r:id="rId55" ref="E77"/>
-    <hyperlink r:id="rId55" ref="E78"/>
+    <hyperlink r:id="rId56" ref="E77"/>
+    <hyperlink r:id="rId56" ref="E78"/>
     <hyperlink r:id="rId56" ref="E79"/>
     <hyperlink r:id="rId57" ref="E80"/>
     <hyperlink r:id="rId58" ref="E81"/>
+    <hyperlink r:id="rId59" ref="E82"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Added details for Antisyphon Red Team Summit 2025
</commit_message>
<xml_diff>
--- a/training_certs_record.xlsx
+++ b/training_certs_record.xlsx
@@ -16,7 +16,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="254">
+  <si>
+    <t xml:space="preserve">Red Team Summit 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antisyphon Training</t>
+  </si>
+  <si>
+    <t>https://api.accredible.com/v1/auth/invite?code=c6b0e9bd58d09168ff4b&amp;credential_id=7a75a750-866f-43fa-9b23-2d937c4e8bf4&amp;url=https%3A%2F%2Fwww.credential.net%2F7a75a750-866f-43fa-9b23-2d937c4e8bf4&amp;ident=34b8ead6-6a2d-4962-b856-ddefc4afba87</t>
+  </si>
   <si>
     <t xml:space="preserve">AWS Educate Introduction to Cloud 101</t>
   </si>
@@ -346,9 +355,6 @@
   </si>
   <si>
     <t xml:space="preserve">Antisyphon Blue Team Summit 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antisyphon Training</t>
   </si>
   <si>
     <t>https://drive.google.com/file/d/1mXGeTD4P_jGjliMg_JVuH19HEiQaOK9M/view?usp=drivesdk</t>
@@ -818,8 +824,11 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1348,7 +1357,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1363,16 +1372,17 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="3">
         <v>45717</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1383,41 +1393,38 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>45717</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5">
         <v>45689</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4">
-        <v>45627</v>
-      </c>
-      <c r="D4" s="1">
-        <v>127699968</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1428,7 +1435,13 @@
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5">
+        <v>45627</v>
+      </c>
+      <c r="D5" s="1">
+        <v>127699968</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1437,65 +1450,59 @@
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1504,27 +1511,27 @@
         <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>18</v>
+      <c r="E11" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
@@ -1532,63 +1539,63 @@
         <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" ht="42.75">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="3" t="s">
+    </row>
+    <row r="15" ht="42.75">
+      <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="E15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="3" t="s">
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" ht="28.5">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="1">
-        <v>8835432</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1597,29 +1604,32 @@
         <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D17" s="1">
+        <v>8835432</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" ht="28.5">
+      <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1">
         <v>8835521</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1630,7 +1640,10 @@
       <c r="B19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1641,55 +1654,52 @@
       <c r="B20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>53</v>
+      <c r="C20" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>62</v>
+      <c r="C22" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>67</v>
@@ -1697,128 +1707,131 @@
       <c r="D24" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="3" t="s">
         <v>71</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="E27" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="D27" s="1">
-        <v>100019282</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="3" t="s">
         <v>80</v>
+      </c>
+      <c r="D28" s="1">
+        <v>100019282</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="E32" s="4" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1830,60 +1843,57 @@
         <v>98</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="3" t="s">
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" ht="27">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" ht="27">
       <c r="A35" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="E35" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="4" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1892,29 +1902,29 @@
         <v>112</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="4" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1923,283 +1933,283 @@
         <v>117</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="D39" s="1">
-        <v>908449736</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="D40" s="1">
+        <v>908449736</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="E41" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="E43" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="1" t="s">
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="C44" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="44" ht="28.5">
-      <c r="A44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="E44" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="45" ht="28.5">
       <c r="A45" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="46" ht="28.5">
       <c r="A46" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="E46" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="1" t="s">
+    </row>
+    <row r="47" ht="28.5">
+      <c r="A47" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="C47" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="E47" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C47" s="1" t="s">
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D47" s="1">
+      <c r="B48" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="1">
         <v>1246352</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="48" ht="28.5">
-      <c r="A48" s="1" t="s">
+      <c r="E48" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" ht="28.5">
+      <c r="A49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1246352</v>
+      <c r="E49" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1246352</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="E51" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="D51" s="1">
-        <v>1246352</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="D52" s="1">
+        <v>1246352</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="C53" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D53" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="E54" s="4" t="s">
         <v>172</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D55" s="1">
-        <v>2350911</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="C56" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D56" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2350911</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2208,91 +2218,94 @@
         <v>180</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="C58" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D58" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E58" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="E59" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="E61" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C62" s="1" t="s">
+      <c r="E62" s="4" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2301,12 +2314,9 @@
         <v>199</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>181</v>
+        <v>58</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E63" s="3" t="s">
         <v>200</v>
       </c>
     </row>
@@ -2315,35 +2325,38 @@
         <v>201</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E64" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>165</v>
+        <v>203</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D65" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="67">
@@ -2354,45 +2367,42 @@
         <v>209</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E70" s="3" t="s">
+      <c r="E70" s="4" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2401,9 +2411,12 @@
         <v>217</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>207</v>
+        <v>130</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2412,60 +2425,54 @@
         <v>219</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="E74" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D74" s="1">
-        <v>46292805</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="D75" s="1">
-        <v>46873384</v>
-      </c>
-      <c r="E75" s="3" t="s">
+        <v>46292805</v>
+      </c>
+      <c r="E75" s="4" t="s">
         <v>229</v>
       </c>
     </row>
@@ -2474,50 +2481,50 @@
         <v>230</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>181</v>
+        <v>227</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D76" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D76" s="1">
+        <v>46873384</v>
+      </c>
+      <c r="E76" s="4" t="s">
         <v>231</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D77" s="1" t="s">
+      <c r="E77" s="4" t="s">
         <v>234</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D78" s="1" t="s">
+      <c r="E78" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="79">
@@ -2525,16 +2532,16 @@
         <v>238</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E79" s="3" t="s">
-        <v>235</v>
+      <c r="E79" s="4" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="80">
@@ -2542,67 +2549,84 @@
         <v>240</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>243</v>
+      <c r="E80" s="4" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="E81" s="4" t="s">
         <v>245</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="E82" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D82" s="1" t="s">
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="B83" s="1" t="s">
         <v>251</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="E1"/>
-    <hyperlink r:id="rId2" ref="E3"/>
+    <hyperlink r:id="rId2" ref="E2"/>
     <hyperlink r:id="rId3" ref="E4"/>
-    <hyperlink r:id="rId4" ref="E8"/>
+    <hyperlink r:id="rId4" ref="E5"/>
     <hyperlink r:id="rId5" ref="E9"/>
     <hyperlink r:id="rId6" ref="E10"/>
-    <hyperlink r:id="rId7" ref="E12"/>
+    <hyperlink r:id="rId7" ref="E11"/>
     <hyperlink r:id="rId8" ref="E13"/>
     <hyperlink r:id="rId9" ref="E14"/>
     <hyperlink r:id="rId10" ref="E15"/>
     <hyperlink r:id="rId11" ref="E16"/>
     <hyperlink r:id="rId12" ref="E17"/>
-    <hyperlink r:id="rId13" ref="E22"/>
+    <hyperlink r:id="rId13" ref="E18"/>
     <hyperlink r:id="rId14" ref="E23"/>
     <hyperlink r:id="rId15" ref="E24"/>
     <hyperlink r:id="rId16" ref="E25"/>
@@ -2612,45 +2636,46 @@
     <hyperlink r:id="rId20" ref="E29"/>
     <hyperlink r:id="rId21" ref="E30"/>
     <hyperlink r:id="rId22" ref="E31"/>
-    <hyperlink r:id="rId23" ref="E33"/>
-    <hyperlink r:id="rId24" ref="D34"/>
-    <hyperlink r:id="rId25" ref="E34"/>
+    <hyperlink r:id="rId23" ref="E32"/>
+    <hyperlink r:id="rId24" ref="E34"/>
+    <hyperlink r:id="rId25" ref="D35"/>
     <hyperlink r:id="rId26" ref="E35"/>
     <hyperlink r:id="rId27" ref="E36"/>
     <hyperlink r:id="rId28" ref="E37"/>
     <hyperlink r:id="rId29" ref="E38"/>
     <hyperlink r:id="rId30" ref="E39"/>
     <hyperlink r:id="rId31" ref="E40"/>
-    <hyperlink r:id="rId32" ref="E42"/>
+    <hyperlink r:id="rId32" ref="E41"/>
     <hyperlink r:id="rId33" ref="E43"/>
     <hyperlink r:id="rId34" ref="E44"/>
     <hyperlink r:id="rId35" ref="E45"/>
     <hyperlink r:id="rId36" ref="E46"/>
     <hyperlink r:id="rId37" ref="E47"/>
     <hyperlink r:id="rId38" ref="E48"/>
-    <hyperlink r:id="rId39" ref="E50"/>
+    <hyperlink r:id="rId39" ref="E49"/>
     <hyperlink r:id="rId40" ref="E51"/>
-    <hyperlink r:id="rId41" ref="E53"/>
-    <hyperlink r:id="rId42" ref="E55"/>
-    <hyperlink r:id="rId43" ref="E57"/>
+    <hyperlink r:id="rId41" ref="E52"/>
+    <hyperlink r:id="rId42" ref="E54"/>
+    <hyperlink r:id="rId43" ref="E56"/>
     <hyperlink r:id="rId44" ref="E58"/>
     <hyperlink r:id="rId45" ref="E59"/>
     <hyperlink r:id="rId46" ref="E60"/>
     <hyperlink r:id="rId47" ref="E61"/>
-    <hyperlink r:id="rId48" ref="E63"/>
-    <hyperlink r:id="rId49" ref="E67"/>
-    <hyperlink r:id="rId50" ref="E69"/>
+    <hyperlink r:id="rId48" ref="E62"/>
+    <hyperlink r:id="rId49" ref="E64"/>
+    <hyperlink r:id="rId50" ref="E68"/>
     <hyperlink r:id="rId51" ref="E70"/>
-    <hyperlink r:id="rId52" ref="E73"/>
+    <hyperlink r:id="rId52" ref="E71"/>
     <hyperlink r:id="rId53" ref="E74"/>
     <hyperlink r:id="rId54" ref="E75"/>
     <hyperlink r:id="rId55" ref="E76"/>
     <hyperlink r:id="rId56" ref="E77"/>
-    <hyperlink r:id="rId56" ref="E78"/>
-    <hyperlink r:id="rId56" ref="E79"/>
+    <hyperlink r:id="rId57" ref="E78"/>
+    <hyperlink r:id="rId57" ref="E79"/>
     <hyperlink r:id="rId57" ref="E80"/>
     <hyperlink r:id="rId58" ref="E81"/>
     <hyperlink r:id="rId59" ref="E82"/>
+    <hyperlink r:id="rId60" ref="E83"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Added cert for AI in Cybersec training conducted by CyberFrat
</commit_message>
<xml_diff>
--- a/training_certs_record.xlsx
+++ b/training_certs_record.xlsx
@@ -16,7 +16,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="258">
+  <si>
+    <t xml:space="preserve">AI in Cybersecurity</t>
+  </si>
+  <si>
+    <t>CyberFrat</t>
+  </si>
+  <si>
+    <t>qjHyOanWrv</t>
+  </si>
+  <si>
+    <t>https://verify.netcredential.com/qjHyOanWrv</t>
+  </si>
   <si>
     <t xml:space="preserve">Red Team Summit 2025</t>
   </si>
@@ -1357,7 +1369,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1381,54 +1393,54 @@
       <c r="C1" s="3">
         <v>45717</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="42.75">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="5">
         <v>45717</v>
       </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5">
         <v>45717</v>
       </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5">
-        <v>45689</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1436,70 +1448,70 @@
         <v>13</v>
       </c>
       <c r="C5" s="5">
-        <v>45627</v>
-      </c>
-      <c r="D5" s="1">
-        <v>127699968</v>
+        <v>45689</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="C6" s="5">
+        <v>45627</v>
+      </c>
+      <c r="D6" s="1">
+        <v>127699968</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1511,72 +1523,72 @@
         <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" ht="42.75">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>40</v>
@@ -1585,7 +1597,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="42.75">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -1593,13 +1605,16 @@
         <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" ht="28.5">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -1607,101 +1622,101 @@
         <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="1">
-        <v>8835432</v>
+        <v>48</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" ht="28.5">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1">
+        <v>8835432</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" ht="28.5">
+      <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="1">
         <v>8835521</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>53</v>
+      <c r="E19" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="5" t="s">
         <v>56</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>65</v>
+      <c r="C23" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1713,58 +1728,55 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="E27" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D28" s="1">
-        <v>100019282</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>81</v>
@@ -1775,41 +1787,41 @@
         <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="D29" s="1">
+        <v>100019282</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>91</v>
@@ -1826,7 +1838,7 @@
         <v>94</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>95</v>
@@ -1843,134 +1855,134 @@
         <v>98</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>99</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="35" ht="27">
+    <row r="35">
       <c r="A35" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E35" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="36">
+      <c r="E35" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" ht="27">
       <c r="A36" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D40" s="1">
-        <v>908449736</v>
+        <v>113</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" s="1" t="s">
         <v>124</v>
+      </c>
+      <c r="D41" s="1">
+        <v>908449736</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>125</v>
@@ -1983,53 +1995,53 @@
       <c r="B42" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>128</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C43" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="C43" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E44" s="4" t="s">
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="45" ht="28.5">
-      <c r="A45" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>141</v>
@@ -2043,53 +2055,53 @@
         <v>143</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="D46" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" ht="28.5">
       <c r="A47" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E47" s="4" t="s">
+    </row>
+    <row r="48" ht="28.5">
+      <c r="A48" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1246352</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="49" ht="28.5">
+    <row r="49">
       <c r="A49" s="1" t="s">
         <v>155</v>
       </c>
@@ -2097,44 +2109,44 @@
         <v>156</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D49" s="1" t="s">
         <v>157</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1246352</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" ht="28.5">
       <c r="A50" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1246352</v>
+        <v>157</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1246352</v>
       </c>
     </row>
     <row r="52">
@@ -2142,57 +2154,60 @@
         <v>164</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D52" s="1">
-        <v>1246352</v>
+      <c r="D52" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="D53" s="1">
+        <v>1246352</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="4" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2204,69 +2219,66 @@
         <v>178</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D56" s="1">
-        <v>2350911</v>
-      </c>
-      <c r="E56" s="4" t="s">
         <v>179</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
+      </c>
+      <c r="D57" s="1">
+        <v>2350911</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>190</v>
@@ -2280,27 +2292,27 @@
         <v>192</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>197</v>
@@ -2314,149 +2326,149 @@
         <v>199</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>58</v>
+        <v>200</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>200</v>
+        <v>179</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>183</v>
+        <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>205</v>
+      <c r="E65" s="4" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>167</v>
+        <v>207</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="C67" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>209</v>
+        <v>134</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>220</v>
+        <v>210</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D74" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="75">
@@ -2467,10 +2479,10 @@
         <v>227</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="D75" s="1">
-        <v>46292805</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>229</v>
@@ -2481,101 +2493,101 @@
         <v>230</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D76" s="1">
-        <v>46873384</v>
+        <v>46292805</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>233</v>
+      <c r="D77" s="1">
+        <v>46873384</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D80" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E80" s="4" t="s">
         <v>241</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>243</v>
+        <v>187</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>120</v>
+        <v>179</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="82">
@@ -2586,7 +2598,7 @@
         <v>247</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>175</v>
+        <v>124</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>248</v>
@@ -2603,31 +2615,48 @@
         <v>251</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>252</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>253</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="E1"/>
     <hyperlink r:id="rId2" ref="E2"/>
-    <hyperlink r:id="rId3" ref="E4"/>
+    <hyperlink r:id="rId3" ref="E3"/>
     <hyperlink r:id="rId4" ref="E5"/>
-    <hyperlink r:id="rId5" ref="E9"/>
+    <hyperlink r:id="rId5" ref="E6"/>
     <hyperlink r:id="rId6" ref="E10"/>
     <hyperlink r:id="rId7" ref="E11"/>
-    <hyperlink r:id="rId8" ref="E13"/>
+    <hyperlink r:id="rId8" ref="E12"/>
     <hyperlink r:id="rId9" ref="E14"/>
     <hyperlink r:id="rId10" ref="E15"/>
     <hyperlink r:id="rId11" ref="E16"/>
     <hyperlink r:id="rId12" ref="E17"/>
     <hyperlink r:id="rId13" ref="E18"/>
-    <hyperlink r:id="rId14" ref="E23"/>
+    <hyperlink r:id="rId14" ref="E19"/>
     <hyperlink r:id="rId15" ref="E24"/>
     <hyperlink r:id="rId16" ref="E25"/>
     <hyperlink r:id="rId17" ref="E26"/>
@@ -2637,45 +2666,46 @@
     <hyperlink r:id="rId21" ref="E30"/>
     <hyperlink r:id="rId22" ref="E31"/>
     <hyperlink r:id="rId23" ref="E32"/>
-    <hyperlink r:id="rId24" ref="E34"/>
-    <hyperlink r:id="rId25" ref="D35"/>
-    <hyperlink r:id="rId26" ref="E35"/>
+    <hyperlink r:id="rId24" ref="E33"/>
+    <hyperlink r:id="rId25" ref="E35"/>
+    <hyperlink r:id="rId26" ref="D36"/>
     <hyperlink r:id="rId27" ref="E36"/>
     <hyperlink r:id="rId28" ref="E37"/>
     <hyperlink r:id="rId29" ref="E38"/>
     <hyperlink r:id="rId30" ref="E39"/>
     <hyperlink r:id="rId31" ref="E40"/>
     <hyperlink r:id="rId32" ref="E41"/>
-    <hyperlink r:id="rId33" ref="E43"/>
+    <hyperlink r:id="rId33" ref="E42"/>
     <hyperlink r:id="rId34" ref="E44"/>
     <hyperlink r:id="rId35" ref="E45"/>
     <hyperlink r:id="rId36" ref="E46"/>
     <hyperlink r:id="rId37" ref="E47"/>
     <hyperlink r:id="rId38" ref="E48"/>
     <hyperlink r:id="rId39" ref="E49"/>
-    <hyperlink r:id="rId40" ref="E51"/>
+    <hyperlink r:id="rId40" ref="E50"/>
     <hyperlink r:id="rId41" ref="E52"/>
-    <hyperlink r:id="rId42" ref="E54"/>
-    <hyperlink r:id="rId43" ref="E56"/>
-    <hyperlink r:id="rId44" ref="E58"/>
+    <hyperlink r:id="rId42" ref="E53"/>
+    <hyperlink r:id="rId43" ref="E55"/>
+    <hyperlink r:id="rId44" ref="E57"/>
     <hyperlink r:id="rId45" ref="E59"/>
     <hyperlink r:id="rId46" ref="E60"/>
     <hyperlink r:id="rId47" ref="E61"/>
     <hyperlink r:id="rId48" ref="E62"/>
-    <hyperlink r:id="rId49" ref="E64"/>
-    <hyperlink r:id="rId50" ref="E68"/>
-    <hyperlink r:id="rId51" ref="E70"/>
+    <hyperlink r:id="rId49" ref="E63"/>
+    <hyperlink r:id="rId50" ref="E65"/>
+    <hyperlink r:id="rId51" ref="E69"/>
     <hyperlink r:id="rId52" ref="E71"/>
-    <hyperlink r:id="rId53" ref="E74"/>
+    <hyperlink r:id="rId53" ref="E72"/>
     <hyperlink r:id="rId54" ref="E75"/>
     <hyperlink r:id="rId55" ref="E76"/>
     <hyperlink r:id="rId56" ref="E77"/>
     <hyperlink r:id="rId57" ref="E78"/>
-    <hyperlink r:id="rId57" ref="E79"/>
-    <hyperlink r:id="rId57" ref="E80"/>
+    <hyperlink r:id="rId58" ref="E79"/>
+    <hyperlink r:id="rId58" ref="E80"/>
     <hyperlink r:id="rId58" ref="E81"/>
     <hyperlink r:id="rId59" ref="E82"/>
     <hyperlink r:id="rId60" ref="E83"/>
+    <hyperlink r:id="rId61" ref="E84"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Added entry for Google's Adversarial Nibbler
</commit_message>
<xml_diff>
--- a/training_certs_record.xlsx
+++ b/training_certs_record.xlsx
@@ -16,7 +16,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="261">
+  <si>
+    <t xml:space="preserve">Google's Adversarial Nibbler Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google, L.P.U. School of Computer Science and Engineering</t>
+  </si>
+  <si>
+    <t>https://media.licdn.com/dms/image/v2/D562DAQHQ6BW5BopEQQ/profile-treasury-image-shrink_800_800/B56ZbacpgmH4Ag-/0/1747421666053?e=1748109600&amp;v=beta&amp;t=y2LZpLWat8rtW0mdG7eq9pJ-KaR6P-Z76VCHdLXot4U</t>
+  </si>
   <si>
     <t xml:space="preserve">AI in Cybersecurity</t>
   </si>
@@ -1369,7 +1378,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="100" workbookViewId="0">
       <selection activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1391,31 +1400,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="3">
-        <v>45717</v>
-      </c>
-      <c r="D1" s="1" t="s">
+        <v>45658</v>
+      </c>
+      <c r="D1" s="1">
+        <v>376081</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" ht="42.75">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="5">
         <v>45717</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="14.25">
+    <row r="3" ht="42.75">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1425,6 +1436,7 @@
       <c r="C3" s="5">
         <v>45717</v>
       </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1439,36 +1451,33 @@
       <c r="C4" s="5">
         <v>45717</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="5">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5">
         <v>45689</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="5">
-        <v>45627</v>
-      </c>
-      <c r="D6" s="1">
-        <v>127699968</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>18</v>
@@ -1481,7 +1490,13 @@
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5">
+        <v>45627</v>
+      </c>
+      <c r="D7" s="1">
+        <v>127699968</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1490,60 +1505,54 @@
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>32</v>
@@ -1557,27 +1566,27 @@
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>25</v>
+      <c r="E13" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
@@ -1585,10 +1594,10 @@
         <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>40</v>
@@ -1597,49 +1606,49 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" ht="42.75">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="4" t="s">
+    </row>
+    <row r="17" ht="42.75">
+      <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="4" t="s">
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" ht="28.5">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="1">
-        <v>8835432</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>52</v>
@@ -1650,29 +1659,32 @@
         <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="D19" s="1">
+        <v>8835432</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" ht="28.5">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1">
         <v>8835521</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1683,7 +1695,10 @@
       <c r="B21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1695,54 +1710,51 @@
         <v>62</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>69</v>
+      <c r="C24" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>74</v>
@@ -1756,27 +1768,27 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>81</v>
@@ -1784,94 +1796,97 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="E29" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="D29" s="1">
-        <v>100019282</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="D30" s="1">
+        <v>100019282</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="E34" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1883,75 +1898,69 @@
         <v>105</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D35" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E35" s="4" t="s">
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="36" ht="27">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" ht="27">
       <c r="A37" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="E37" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>113</v>
+      <c r="D38" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>120</v>
@@ -1962,27 +1971,27 @@
         <v>121</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D41" s="1">
-        <v>908449736</v>
+        <v>116</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>125</v>
@@ -1993,26 +2002,32 @@
         <v>126</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="1">
+        <v>908449736</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="E43" s="4" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2023,59 +2038,53 @@
       <c r="B44" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="E45" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="1" t="s">
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="B46" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="46" ht="28.5">
-      <c r="A46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="47" ht="28.5">
       <c r="A47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="C47" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>148</v>
@@ -2089,95 +2098,95 @@
         <v>150</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="E48" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D48" s="1" t="s">
+    </row>
+    <row r="49" ht="28.5">
+      <c r="A49" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="B49" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="E49" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D49" s="1">
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D50" s="1">
         <v>1246352</v>
       </c>
-      <c r="E49" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="50" ht="28.5">
-      <c r="A50" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="E50" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" ht="28.5">
+      <c r="A51" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D51" s="1">
-        <v>1246352</v>
+      <c r="D51" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1246352</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D53" s="1">
-        <v>1246352</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>170</v>
@@ -2188,9 +2197,15 @@
         <v>171</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1">
+        <v>1246352</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2199,15 +2214,9 @@
         <v>174</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>127</v>
+        <v>175</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E55" s="4" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2216,29 +2225,29 @@
         <v>177</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="E56" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D57" s="1">
-        <v>2350911</v>
-      </c>
-      <c r="E57" s="4" t="s">
+      <c r="D57" s="1" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2247,26 +2256,29 @@
         <v>184</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
+      </c>
+      <c r="D58" s="1">
+        <v>2350911</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E59" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2275,13 +2287,10 @@
         <v>189</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>191</v>
@@ -2292,27 +2301,27 @@
         <v>192</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D61" s="1" t="s">
+      <c r="E61" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="C62" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>197</v>
@@ -2326,91 +2335,94 @@
         <v>199</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="C64" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>204</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>187</v>
+        <v>65</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="E66" s="4" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>171</v>
+        <v>210</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>210</v>
+      <c r="D68" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="70">
@@ -2418,21 +2430,24 @@
         <v>217</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>210</v>
+      <c r="E70" s="4" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="72">
@@ -2440,100 +2455,94 @@
         <v>221</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>224</v>
+      <c r="E73" s="4" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="E76" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="D76" s="1">
-        <v>46292805</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="C77" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D77" s="1">
-        <v>46873384</v>
+        <v>46292805</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
+      </c>
+      <c r="D78" s="1">
+        <v>46873384</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>238</v>
@@ -2544,10 +2553,10 @@
         <v>239</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>240</v>
@@ -2561,84 +2570,101 @@
         <v>242</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>243</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E81" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>247</v>
+        <v>190</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>124</v>
+        <v>182</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>248</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D83" s="1" t="s">
+      <c r="E83" s="4" t="s">
         <v>252</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D84" s="1" t="s">
+      <c r="E84" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="E84" s="4" t="s">
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
         <v>257</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -2646,18 +2672,18 @@
     <hyperlink r:id="rId1" ref="E1"/>
     <hyperlink r:id="rId2" ref="E2"/>
     <hyperlink r:id="rId3" ref="E3"/>
-    <hyperlink r:id="rId4" ref="E5"/>
+    <hyperlink r:id="rId4" ref="E4"/>
     <hyperlink r:id="rId5" ref="E6"/>
-    <hyperlink r:id="rId6" ref="E10"/>
+    <hyperlink r:id="rId6" ref="E7"/>
     <hyperlink r:id="rId7" ref="E11"/>
     <hyperlink r:id="rId8" ref="E12"/>
-    <hyperlink r:id="rId9" ref="E14"/>
+    <hyperlink r:id="rId9" ref="E13"/>
     <hyperlink r:id="rId10" ref="E15"/>
     <hyperlink r:id="rId11" ref="E16"/>
     <hyperlink r:id="rId12" ref="E17"/>
     <hyperlink r:id="rId13" ref="E18"/>
     <hyperlink r:id="rId14" ref="E19"/>
-    <hyperlink r:id="rId15" ref="E24"/>
+    <hyperlink r:id="rId15" ref="E20"/>
     <hyperlink r:id="rId16" ref="E25"/>
     <hyperlink r:id="rId17" ref="E26"/>
     <hyperlink r:id="rId18" ref="E27"/>
@@ -2667,45 +2693,46 @@
     <hyperlink r:id="rId22" ref="E31"/>
     <hyperlink r:id="rId23" ref="E32"/>
     <hyperlink r:id="rId24" ref="E33"/>
-    <hyperlink r:id="rId25" ref="E35"/>
-    <hyperlink r:id="rId26" ref="D36"/>
-    <hyperlink r:id="rId27" ref="E36"/>
+    <hyperlink r:id="rId25" ref="E34"/>
+    <hyperlink r:id="rId26" ref="E36"/>
+    <hyperlink r:id="rId27" ref="D37"/>
     <hyperlink r:id="rId28" ref="E37"/>
     <hyperlink r:id="rId29" ref="E38"/>
     <hyperlink r:id="rId30" ref="E39"/>
     <hyperlink r:id="rId31" ref="E40"/>
     <hyperlink r:id="rId32" ref="E41"/>
     <hyperlink r:id="rId33" ref="E42"/>
-    <hyperlink r:id="rId34" ref="E44"/>
+    <hyperlink r:id="rId34" ref="E43"/>
     <hyperlink r:id="rId35" ref="E45"/>
     <hyperlink r:id="rId36" ref="E46"/>
     <hyperlink r:id="rId37" ref="E47"/>
     <hyperlink r:id="rId38" ref="E48"/>
     <hyperlink r:id="rId39" ref="E49"/>
     <hyperlink r:id="rId40" ref="E50"/>
-    <hyperlink r:id="rId41" ref="E52"/>
+    <hyperlink r:id="rId41" ref="E51"/>
     <hyperlink r:id="rId42" ref="E53"/>
-    <hyperlink r:id="rId43" ref="E55"/>
-    <hyperlink r:id="rId44" ref="E57"/>
-    <hyperlink r:id="rId45" ref="E59"/>
+    <hyperlink r:id="rId43" ref="E54"/>
+    <hyperlink r:id="rId44" ref="E56"/>
+    <hyperlink r:id="rId45" ref="E58"/>
     <hyperlink r:id="rId46" ref="E60"/>
     <hyperlink r:id="rId47" ref="E61"/>
     <hyperlink r:id="rId48" ref="E62"/>
     <hyperlink r:id="rId49" ref="E63"/>
-    <hyperlink r:id="rId50" ref="E65"/>
-    <hyperlink r:id="rId51" ref="E69"/>
-    <hyperlink r:id="rId52" ref="E71"/>
+    <hyperlink r:id="rId50" ref="E64"/>
+    <hyperlink r:id="rId51" ref="E66"/>
+    <hyperlink r:id="rId52" ref="E70"/>
     <hyperlink r:id="rId53" ref="E72"/>
-    <hyperlink r:id="rId54" ref="E75"/>
+    <hyperlink r:id="rId54" ref="E73"/>
     <hyperlink r:id="rId55" ref="E76"/>
     <hyperlink r:id="rId56" ref="E77"/>
     <hyperlink r:id="rId57" ref="E78"/>
     <hyperlink r:id="rId58" ref="E79"/>
-    <hyperlink r:id="rId58" ref="E80"/>
-    <hyperlink r:id="rId58" ref="E81"/>
+    <hyperlink r:id="rId59" ref="E80"/>
+    <hyperlink r:id="rId59" ref="E81"/>
     <hyperlink r:id="rId59" ref="E82"/>
     <hyperlink r:id="rId60" ref="E83"/>
     <hyperlink r:id="rId61" ref="E84"/>
+    <hyperlink r:id="rId62" ref="E85"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Added entry for OSINTCon 2025, fixed entry for Linux summer training
</commit_message>
<xml_diff>
--- a/training_certs_record.xlsx
+++ b/training_certs_record.xlsx
@@ -16,7 +16,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="266">
+  <si>
+    <t xml:space="preserve">OSINTCon 2025 - Participant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSINTCon 2025</t>
+  </si>
+  <si>
+    <t>ef5b8f85-d374-4385-8578-0028933ad08e</t>
+  </si>
+  <si>
+    <t>https://credsverse.com/credentials/ef5b8f85-d374-4385-8578-0028933ad08e</t>
+  </si>
   <si>
     <t xml:space="preserve">Google's Adversarial Nibbler Project</t>
   </si>
@@ -100,6 +112,9 @@
   </si>
   <si>
     <t xml:space="preserve">Summer Training on Linux System Administration - LPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L.P.U. Centre of Professional Excellence</t>
   </si>
   <si>
     <t xml:space="preserve">July 2024</t>
@@ -814,13 +829,13 @@
     </font>
     <font>
       <u/>
-      <sz val="11.000000"/>
+      <sz val="10.000000"/>
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="10.000000"/>
+      <sz val="11.000000"/>
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
@@ -845,11 +860,8 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -859,13 +871,13 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="17" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1378,7 +1390,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1393,363 +1405,366 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="2">
+        <v>45809</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="42.75">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
         <v>45658</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D2" s="1">
         <v>376081</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5">
-        <v>45717</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="42.75">
+    <row r="3" ht="14.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="2">
         <v>45717</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" ht="42.75">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
         <v>45717</v>
       </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="5">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
         <v>45717</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5">
-        <v>45689</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="C6" s="2">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="5">
-        <v>45627</v>
-      </c>
-      <c r="D7" s="1">
-        <v>127699968</v>
+      <c r="C7" s="2">
+        <v>45689</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="C8" s="2">
+        <v>45627</v>
+      </c>
+      <c r="D8" s="1">
+        <v>127699968</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="B12" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" ht="42.75">
-      <c r="A17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" ht="42.75">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" ht="28.5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="1">
-        <v>8835432</v>
+        <v>56</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" ht="28.5">
       <c r="A20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="D20" s="1">
-        <v>8835521</v>
+        <v>8835432</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" ht="28.5">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="D21" s="1">
+        <v>8835521</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>63</v>
+        <v>70</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26">
@@ -1759,98 +1774,98 @@
       <c r="B26" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="C26" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="D26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>83</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="1">
-        <v>100019282</v>
+      <c r="D30" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
+      </c>
+      <c r="D31" s="1">
+        <v>100019282</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>95</v>
@@ -1864,91 +1879,91 @@
         <v>97</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" ht="27">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38">
+      <c r="D37" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" ht="27">
       <c r="A38" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>115</v>
+        <v>67</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="3" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1957,105 +1972,105 @@
         <v>119</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="E40" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D42" s="1">
-        <v>908449736</v>
+        <v>121</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="D43" s="1">
+        <v>908449736</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C44" s="5" t="s">
         <v>135</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D45" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="C45" s="2" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2076,7 +2091,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" ht="28.5">
+    <row r="47">
       <c r="A47" s="1" t="s">
         <v>146</v>
       </c>
@@ -2084,41 +2099,41 @@
         <v>147</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" ht="28.5">
       <c r="A48" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" ht="28.5">
       <c r="A49" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>156</v>
@@ -2127,7 +2142,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" ht="28.5">
       <c r="A50" s="1" t="s">
         <v>158</v>
       </c>
@@ -2137,534 +2152,551 @@
       <c r="C50" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D51" s="1">
         <v>1246352</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="51" ht="28.5">
-      <c r="A51" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="E51" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="52" ht="28.5">
+      <c r="A52" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1246352</v>
+      <c r="D52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1246352</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D54" s="1">
-        <v>1246352</v>
+        <v>173</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1246352</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>183</v>
       </c>
+      <c r="E57" s="4" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D58" s="1">
-        <v>2350911</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>188</v>
+      <c r="D59" s="1">
+        <v>2350911</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>65</v>
+        <v>208</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>207</v>
+        <v>187</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>190</v>
+        <v>70</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>212</v>
       </c>
+      <c r="E67" s="4" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>213</v>
+        <v>218</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>213</v>
+        <v>218</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>223</v>
+      <c r="C72" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>216</v>
+        <v>142</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E76" s="4" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D77" s="1">
-        <v>46292805</v>
+        <v>232</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="D78" s="1">
-        <v>46873384</v>
+        <v>46292805</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="C79" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D79" s="1" t="s">
         <v>240</v>
       </c>
+      <c r="D79" s="1">
+        <v>46873384</v>
+      </c>
       <c r="E79" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E83" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2673,18 +2705,18 @@
     <hyperlink r:id="rId2" ref="E2"/>
     <hyperlink r:id="rId3" ref="E3"/>
     <hyperlink r:id="rId4" ref="E4"/>
-    <hyperlink r:id="rId5" ref="E6"/>
+    <hyperlink r:id="rId5" ref="E5"/>
     <hyperlink r:id="rId6" ref="E7"/>
-    <hyperlink r:id="rId7" ref="E11"/>
+    <hyperlink r:id="rId7" ref="E8"/>
     <hyperlink r:id="rId8" ref="E12"/>
     <hyperlink r:id="rId9" ref="E13"/>
-    <hyperlink r:id="rId10" ref="E15"/>
+    <hyperlink r:id="rId10" ref="E14"/>
     <hyperlink r:id="rId11" ref="E16"/>
     <hyperlink r:id="rId12" ref="E17"/>
     <hyperlink r:id="rId13" ref="E18"/>
     <hyperlink r:id="rId14" ref="E19"/>
     <hyperlink r:id="rId15" ref="E20"/>
-    <hyperlink r:id="rId16" ref="E25"/>
+    <hyperlink r:id="rId16" ref="E21"/>
     <hyperlink r:id="rId17" ref="E26"/>
     <hyperlink r:id="rId18" ref="E27"/>
     <hyperlink r:id="rId19" ref="E28"/>
@@ -2694,45 +2726,46 @@
     <hyperlink r:id="rId23" ref="E32"/>
     <hyperlink r:id="rId24" ref="E33"/>
     <hyperlink r:id="rId25" ref="E34"/>
-    <hyperlink r:id="rId26" ref="E36"/>
-    <hyperlink r:id="rId27" ref="D37"/>
-    <hyperlink r:id="rId28" ref="E37"/>
+    <hyperlink r:id="rId26" ref="E35"/>
+    <hyperlink r:id="rId27" ref="E37"/>
+    <hyperlink r:id="rId28" ref="D38"/>
     <hyperlink r:id="rId29" ref="E38"/>
     <hyperlink r:id="rId30" ref="E39"/>
     <hyperlink r:id="rId31" ref="E40"/>
     <hyperlink r:id="rId32" ref="E41"/>
     <hyperlink r:id="rId33" ref="E42"/>
     <hyperlink r:id="rId34" ref="E43"/>
-    <hyperlink r:id="rId35" ref="E45"/>
+    <hyperlink r:id="rId35" ref="E44"/>
     <hyperlink r:id="rId36" ref="E46"/>
     <hyperlink r:id="rId37" ref="E47"/>
     <hyperlink r:id="rId38" ref="E48"/>
     <hyperlink r:id="rId39" ref="E49"/>
     <hyperlink r:id="rId40" ref="E50"/>
     <hyperlink r:id="rId41" ref="E51"/>
-    <hyperlink r:id="rId42" ref="E53"/>
+    <hyperlink r:id="rId42" ref="E52"/>
     <hyperlink r:id="rId43" ref="E54"/>
-    <hyperlink r:id="rId44" ref="E56"/>
-    <hyperlink r:id="rId45" ref="E58"/>
-    <hyperlink r:id="rId46" ref="E60"/>
+    <hyperlink r:id="rId44" ref="E55"/>
+    <hyperlink r:id="rId45" ref="E57"/>
+    <hyperlink r:id="rId46" ref="E59"/>
     <hyperlink r:id="rId47" ref="E61"/>
     <hyperlink r:id="rId48" ref="E62"/>
     <hyperlink r:id="rId49" ref="E63"/>
     <hyperlink r:id="rId50" ref="E64"/>
-    <hyperlink r:id="rId51" ref="E66"/>
-    <hyperlink r:id="rId52" ref="E70"/>
-    <hyperlink r:id="rId53" ref="E72"/>
+    <hyperlink r:id="rId51" ref="E65"/>
+    <hyperlink r:id="rId52" ref="E67"/>
+    <hyperlink r:id="rId53" ref="E71"/>
     <hyperlink r:id="rId54" ref="E73"/>
-    <hyperlink r:id="rId55" ref="E76"/>
+    <hyperlink r:id="rId55" ref="E74"/>
     <hyperlink r:id="rId56" ref="E77"/>
     <hyperlink r:id="rId57" ref="E78"/>
     <hyperlink r:id="rId58" ref="E79"/>
     <hyperlink r:id="rId59" ref="E80"/>
-    <hyperlink r:id="rId59" ref="E81"/>
-    <hyperlink r:id="rId59" ref="E82"/>
+    <hyperlink r:id="rId60" ref="E81"/>
+    <hyperlink r:id="rId60" ref="E82"/>
     <hyperlink r:id="rId60" ref="E83"/>
     <hyperlink r:id="rId61" ref="E84"/>
     <hyperlink r:id="rId62" ref="E85"/>
+    <hyperlink r:id="rId63" ref="E86"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Added an entry for a web sec workshop conducted by Flare
</commit_message>
<xml_diff>
--- a/training_certs_record.xlsx
+++ b/training_certs_record.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -16,7 +16,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
+  <si>
+    <t xml:space="preserve">The Burglar's Guide to Web Application Testing: Stealing Secrets Like a Hobbit</t>
+  </si>
+  <si>
+    <t>Flare</t>
+  </si>
+  <si>
+    <t>3aab5818-6376-4775-96c3-9b7f94663808</t>
+  </si>
+  <si>
+    <t>https://credsverse.com/credentials/3aab5818-6376-4775-96c3-9b7f94663808</t>
+  </si>
   <si>
     <t xml:space="preserve">OSINTCon 2025 - Participant</t>
   </si>
@@ -829,13 +841,13 @@
     </font>
     <font>
       <u/>
-      <sz val="10.000000"/>
+      <sz val="11.000000"/>
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="11.000000"/>
+      <sz val="10.000000"/>
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
@@ -860,8 +872,11 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -871,10 +886,10 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="17" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1390,7 +1405,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1408,172 +1423,175 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
-        <v>45809</v>
+      <c r="C1" s="3">
+        <v>45870</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="42.75">
+    <row r="2" ht="14.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
+        <v>45809</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" ht="42.75">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5">
         <v>45658</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <v>376081</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45717</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="42.75">
+    <row r="4" ht="14.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>45717</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" ht="42.75">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5">
         <v>45717</v>
       </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5">
         <v>45717</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2">
-        <v>45689</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="C7" s="5">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="2">
-        <v>45627</v>
-      </c>
-      <c r="D8" s="1">
-        <v>127699968</v>
+      <c r="C8" s="5">
+        <v>45689</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="C9" s="5">
+        <v>45627</v>
+      </c>
+      <c r="D9" s="1">
+        <v>127699968</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13">
@@ -1584,9 +1602,6 @@
         <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1598,72 +1613,72 @@
         <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" ht="42.75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>52</v>
@@ -1672,7 +1687,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="42.75">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
@@ -1680,13 +1695,16 @@
         <v>55</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" ht="28.5">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -1694,101 +1712,101 @@
         <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="1">
-        <v>8835432</v>
+        <v>60</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" ht="28.5">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D21" s="1">
+        <v>8835432</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" ht="28.5">
+      <c r="A22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="1">
         <v>8835521</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>65</v>
+      <c r="E22" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="2" t="s">
         <v>68</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>77</v>
+      <c r="C26" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1800,58 +1818,55 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="E30" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D31" s="1">
-        <v>100019282</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>93</v>
@@ -1862,41 +1877,41 @@
         <v>94</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
+      </c>
+      <c r="D32" s="1">
+        <v>100019282</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>103</v>
@@ -1913,7 +1928,7 @@
         <v>106</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>107</v>
@@ -1930,134 +1945,134 @@
         <v>110</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>111</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="38" ht="27">
+    <row r="38">
       <c r="A38" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E38" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="39">
+      <c r="E38" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" ht="27">
       <c r="A39" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D43" s="1">
-        <v>908449736</v>
+        <v>125</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D44" s="1" t="s">
         <v>136</v>
+      </c>
+      <c r="D44" s="1">
+        <v>908449736</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>137</v>
@@ -2070,53 +2085,53 @@
       <c r="B45" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>140</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C46" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="C46" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E47" s="4" t="s">
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="48" ht="28.5">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>153</v>
@@ -2130,53 +2145,53 @@
         <v>155</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="D49" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" ht="28.5">
       <c r="A50" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E50" s="4" t="s">
+    </row>
+    <row r="51" ht="28.5">
+      <c r="A51" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="D51" s="1">
-        <v>1246352</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="52" ht="28.5">
+    <row r="52">
       <c r="A52" s="1" t="s">
         <v>167</v>
       </c>
@@ -2184,44 +2199,44 @@
         <v>168</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D52" s="1" t="s">
         <v>169</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1246352</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" ht="28.5">
       <c r="A53" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D53" s="1">
-        <v>1246352</v>
+        <v>169</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>175</v>
+        <v>169</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1246352</v>
       </c>
     </row>
     <row r="55">
@@ -2229,57 +2244,60 @@
         <v>176</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D55" s="1">
-        <v>1246352</v>
+      <c r="D55" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="D56" s="1">
+        <v>1246352</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="4" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2291,69 +2309,66 @@
         <v>190</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D59" s="1">
-        <v>2350911</v>
-      </c>
-      <c r="E59" s="4" t="s">
         <v>191</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
+      </c>
+      <c r="D60" s="1">
+        <v>2350911</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>202</v>
@@ -2367,27 +2382,27 @@
         <v>204</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>209</v>
@@ -2401,149 +2416,149 @@
         <v>211</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>70</v>
+        <v>212</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>212</v>
+        <v>191</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>195</v>
+        <v>74</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>217</v>
+      <c r="E68" s="4" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>179</v>
+        <v>219</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="C70" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>221</v>
+        <v>146</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D77" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="78">
@@ -2554,10 +2569,10 @@
         <v>239</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="D78" s="1">
-        <v>46292805</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>241</v>
@@ -2568,101 +2583,101 @@
         <v>242</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D79" s="1">
-        <v>46873384</v>
+        <v>46292805</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>245</v>
+      <c r="D80" s="1">
+        <v>46873384</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D83" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E83" s="4" t="s">
         <v>253</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>255</v>
+        <v>199</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>132</v>
+        <v>191</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="85">
@@ -2673,7 +2688,7 @@
         <v>259</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>187</v>
+        <v>136</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>260</v>
@@ -2690,13 +2705,30 @@
         <v>263</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>264</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>265</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2706,18 +2738,18 @@
     <hyperlink r:id="rId3" ref="E3"/>
     <hyperlink r:id="rId4" ref="E4"/>
     <hyperlink r:id="rId5" ref="E5"/>
-    <hyperlink r:id="rId6" ref="E7"/>
+    <hyperlink r:id="rId6" ref="E6"/>
     <hyperlink r:id="rId7" ref="E8"/>
-    <hyperlink r:id="rId8" ref="E12"/>
+    <hyperlink r:id="rId8" ref="E9"/>
     <hyperlink r:id="rId9" ref="E13"/>
     <hyperlink r:id="rId10" ref="E14"/>
-    <hyperlink r:id="rId11" ref="E16"/>
+    <hyperlink r:id="rId11" ref="E15"/>
     <hyperlink r:id="rId12" ref="E17"/>
     <hyperlink r:id="rId13" ref="E18"/>
     <hyperlink r:id="rId14" ref="E19"/>
     <hyperlink r:id="rId15" ref="E20"/>
     <hyperlink r:id="rId16" ref="E21"/>
-    <hyperlink r:id="rId17" ref="E26"/>
+    <hyperlink r:id="rId17" ref="E22"/>
     <hyperlink r:id="rId18" ref="E27"/>
     <hyperlink r:id="rId19" ref="E28"/>
     <hyperlink r:id="rId20" ref="E29"/>
@@ -2727,45 +2759,46 @@
     <hyperlink r:id="rId24" ref="E33"/>
     <hyperlink r:id="rId25" ref="E34"/>
     <hyperlink r:id="rId26" ref="E35"/>
-    <hyperlink r:id="rId27" ref="E37"/>
-    <hyperlink r:id="rId28" ref="D38"/>
-    <hyperlink r:id="rId29" ref="E38"/>
+    <hyperlink r:id="rId27" ref="E36"/>
+    <hyperlink r:id="rId28" ref="E38"/>
+    <hyperlink r:id="rId29" ref="D39"/>
     <hyperlink r:id="rId30" ref="E39"/>
     <hyperlink r:id="rId31" ref="E40"/>
     <hyperlink r:id="rId32" ref="E41"/>
     <hyperlink r:id="rId33" ref="E42"/>
     <hyperlink r:id="rId34" ref="E43"/>
     <hyperlink r:id="rId35" ref="E44"/>
-    <hyperlink r:id="rId36" ref="E46"/>
+    <hyperlink r:id="rId36" ref="E45"/>
     <hyperlink r:id="rId37" ref="E47"/>
     <hyperlink r:id="rId38" ref="E48"/>
     <hyperlink r:id="rId39" ref="E49"/>
     <hyperlink r:id="rId40" ref="E50"/>
     <hyperlink r:id="rId41" ref="E51"/>
     <hyperlink r:id="rId42" ref="E52"/>
-    <hyperlink r:id="rId43" ref="E54"/>
+    <hyperlink r:id="rId43" ref="E53"/>
     <hyperlink r:id="rId44" ref="E55"/>
-    <hyperlink r:id="rId45" ref="E57"/>
-    <hyperlink r:id="rId46" ref="E59"/>
-    <hyperlink r:id="rId47" ref="E61"/>
+    <hyperlink r:id="rId45" ref="E56"/>
+    <hyperlink r:id="rId46" ref="E58"/>
+    <hyperlink r:id="rId47" ref="E60"/>
     <hyperlink r:id="rId48" ref="E62"/>
     <hyperlink r:id="rId49" ref="E63"/>
     <hyperlink r:id="rId50" ref="E64"/>
     <hyperlink r:id="rId51" ref="E65"/>
-    <hyperlink r:id="rId52" ref="E67"/>
-    <hyperlink r:id="rId53" ref="E71"/>
-    <hyperlink r:id="rId54" ref="E73"/>
+    <hyperlink r:id="rId52" ref="E66"/>
+    <hyperlink r:id="rId53" ref="E68"/>
+    <hyperlink r:id="rId54" ref="E72"/>
     <hyperlink r:id="rId55" ref="E74"/>
-    <hyperlink r:id="rId56" ref="E77"/>
+    <hyperlink r:id="rId56" ref="E75"/>
     <hyperlink r:id="rId57" ref="E78"/>
     <hyperlink r:id="rId58" ref="E79"/>
     <hyperlink r:id="rId59" ref="E80"/>
     <hyperlink r:id="rId60" ref="E81"/>
-    <hyperlink r:id="rId60" ref="E82"/>
-    <hyperlink r:id="rId60" ref="E83"/>
+    <hyperlink r:id="rId61" ref="E82"/>
+    <hyperlink r:id="rId61" ref="E83"/>
     <hyperlink r:id="rId61" ref="E84"/>
     <hyperlink r:id="rId62" ref="E85"/>
     <hyperlink r:id="rId63" ref="E86"/>
+    <hyperlink r:id="rId64" ref="E87"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
+ I pwned AD Attacks Lab
</commit_message>
<xml_diff>
--- a/training_certs_record.xlsx
+++ b/training_certs_record.xlsx
@@ -16,7 +16,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="274">
+  <si>
+    <t xml:space="preserve">I pwned Active Directory Attacks Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altered Security</t>
+  </si>
+  <si>
+    <t>68b04d94a01104712080e487</t>
+  </si>
+  <si>
+    <t>https://api.eu.badgr.io/public/assertions/h1bTjlwXSPS4qxPW9aic4g</t>
+  </si>
   <si>
     <t xml:space="preserve">The Burglar's Guide to Web Application Testing: Stealing Secrets Like a Hobbit</t>
   </si>
@@ -1436,7 +1448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="14.25">
+    <row r="2" ht="28.5">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1444,16 +1456,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="5">
-        <v>45809</v>
+        <v>45870</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" ht="42.75">
+    <row r="3" ht="14.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1461,33 +1473,33 @@
         <v>9</v>
       </c>
       <c r="C3" s="5">
+        <v>45809</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" ht="42.75">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5">
         <v>45658</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <v>376081</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="5">
-        <v>45717</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" ht="42.75">
+    <row r="5" ht="14.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1497,54 +1509,54 @@
       <c r="C5" s="5">
         <v>45717</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" ht="42.75">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5">
         <v>45717</v>
       </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5">
         <v>45717</v>
       </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="5">
-        <v>45689</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1552,60 +1564,63 @@
         <v>28</v>
       </c>
       <c r="C9" s="5">
-        <v>45627</v>
-      </c>
-      <c r="D9" s="1">
-        <v>127699968</v>
+        <v>45689</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="C10" s="5">
+        <v>45627</v>
+      </c>
+      <c r="D10" s="1">
+        <v>127699968</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14">
@@ -1616,9 +1631,6 @@
         <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1630,72 +1642,72 @@
         <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" ht="42.75">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>56</v>
@@ -1704,7 +1716,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" ht="42.75">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -1712,13 +1724,16 @@
         <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>60</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" ht="28.5">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -1726,101 +1741,101 @@
         <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="1">
-        <v>8835432</v>
+        <v>64</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" ht="28.5">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D22" s="1">
+        <v>8835432</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" ht="28.5">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="1">
         <v>8835521</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>69</v>
+      <c r="E23" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="5" t="s">
         <v>72</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>81</v>
+      <c r="C27" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1832,58 +1847,55 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="E31" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D32" s="1">
-        <v>100019282</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>97</v>
@@ -1894,41 +1906,41 @@
         <v>98</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
+      </c>
+      <c r="D33" s="1">
+        <v>100019282</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>107</v>
@@ -1945,7 +1957,7 @@
         <v>110</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>111</v>
@@ -1962,134 +1974,134 @@
         <v>114</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>115</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E38" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="39" ht="27">
+    <row r="39">
       <c r="A39" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E39" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="40">
+      <c r="E39" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" ht="27">
       <c r="A40" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>124</v>
+        <v>75</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D44" s="1">
-        <v>908449736</v>
+        <v>129</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D45" s="1" t="s">
         <v>140</v>
+      </c>
+      <c r="D45" s="1">
+        <v>908449736</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>141</v>
@@ -2102,53 +2114,53 @@
       <c r="B46" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>144</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C47" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="C47" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E48" s="4" t="s">
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="49" ht="28.5">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>157</v>
@@ -2162,53 +2174,53 @@
         <v>159</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="D50" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" ht="28.5">
       <c r="A51" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E51" s="4" t="s">
+    </row>
+    <row r="52" ht="28.5">
+      <c r="A52" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1246352</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="53" ht="28.5">
+    <row r="53">
       <c r="A53" s="1" t="s">
         <v>171</v>
       </c>
@@ -2216,44 +2228,44 @@
         <v>172</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D53" s="1" t="s">
         <v>173</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1246352</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" ht="28.5">
       <c r="A54" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D54" s="1">
-        <v>1246352</v>
+        <v>173</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>179</v>
+        <v>173</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1246352</v>
       </c>
     </row>
     <row r="56">
@@ -2261,57 +2273,60 @@
         <v>180</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D56" s="1">
-        <v>1246352</v>
+      <c r="D56" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>185</v>
       </c>
+      <c r="D57" s="1">
+        <v>1246352</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="4" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2323,69 +2338,66 @@
         <v>194</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D60" s="1">
-        <v>2350911</v>
-      </c>
-      <c r="E60" s="4" t="s">
         <v>195</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
+      </c>
+      <c r="D61" s="1">
+        <v>2350911</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>206</v>
@@ -2399,27 +2411,27 @@
         <v>208</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>213</v>
@@ -2433,149 +2445,149 @@
         <v>215</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>74</v>
+        <v>216</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>216</v>
+        <v>195</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>199</v>
+        <v>78</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>221</v>
+      <c r="E69" s="4" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>183</v>
+        <v>223</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="C71" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>225</v>
+        <v>150</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D78" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="79">
@@ -2586,10 +2598,10 @@
         <v>243</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="D79" s="1">
-        <v>46292805</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>245</v>
@@ -2600,101 +2612,101 @@
         <v>246</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D80" s="1">
-        <v>46873384</v>
+        <v>46292805</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>249</v>
+      <c r="D81" s="1">
+        <v>46873384</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>191</v>
+        <v>220</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D84" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E84" s="4" t="s">
         <v>257</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>259</v>
+        <v>203</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="86">
@@ -2705,7 +2717,7 @@
         <v>263</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>191</v>
+        <v>140</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>264</v>
@@ -2722,13 +2734,30 @@
         <v>267</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>268</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>269</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2739,18 +2768,18 @@
     <hyperlink r:id="rId4" ref="E4"/>
     <hyperlink r:id="rId5" ref="E5"/>
     <hyperlink r:id="rId6" ref="E6"/>
-    <hyperlink r:id="rId7" ref="E8"/>
+    <hyperlink r:id="rId7" ref="E7"/>
     <hyperlink r:id="rId8" ref="E9"/>
-    <hyperlink r:id="rId9" ref="E13"/>
+    <hyperlink r:id="rId9" ref="E10"/>
     <hyperlink r:id="rId10" ref="E14"/>
     <hyperlink r:id="rId11" ref="E15"/>
-    <hyperlink r:id="rId12" ref="E17"/>
+    <hyperlink r:id="rId12" ref="E16"/>
     <hyperlink r:id="rId13" ref="E18"/>
     <hyperlink r:id="rId14" ref="E19"/>
     <hyperlink r:id="rId15" ref="E20"/>
     <hyperlink r:id="rId16" ref="E21"/>
     <hyperlink r:id="rId17" ref="E22"/>
-    <hyperlink r:id="rId18" ref="E27"/>
+    <hyperlink r:id="rId18" ref="E23"/>
     <hyperlink r:id="rId19" ref="E28"/>
     <hyperlink r:id="rId20" ref="E29"/>
     <hyperlink r:id="rId21" ref="E30"/>
@@ -2760,45 +2789,46 @@
     <hyperlink r:id="rId25" ref="E34"/>
     <hyperlink r:id="rId26" ref="E35"/>
     <hyperlink r:id="rId27" ref="E36"/>
-    <hyperlink r:id="rId28" ref="E38"/>
-    <hyperlink r:id="rId29" ref="D39"/>
-    <hyperlink r:id="rId30" ref="E39"/>
+    <hyperlink r:id="rId28" ref="E37"/>
+    <hyperlink r:id="rId29" ref="E39"/>
+    <hyperlink r:id="rId30" ref="D40"/>
     <hyperlink r:id="rId31" ref="E40"/>
     <hyperlink r:id="rId32" ref="E41"/>
     <hyperlink r:id="rId33" ref="E42"/>
     <hyperlink r:id="rId34" ref="E43"/>
     <hyperlink r:id="rId35" ref="E44"/>
     <hyperlink r:id="rId36" ref="E45"/>
-    <hyperlink r:id="rId37" ref="E47"/>
+    <hyperlink r:id="rId37" ref="E46"/>
     <hyperlink r:id="rId38" ref="E48"/>
     <hyperlink r:id="rId39" ref="E49"/>
     <hyperlink r:id="rId40" ref="E50"/>
     <hyperlink r:id="rId41" ref="E51"/>
     <hyperlink r:id="rId42" ref="E52"/>
     <hyperlink r:id="rId43" ref="E53"/>
-    <hyperlink r:id="rId44" ref="E55"/>
+    <hyperlink r:id="rId44" ref="E54"/>
     <hyperlink r:id="rId45" ref="E56"/>
-    <hyperlink r:id="rId46" ref="E58"/>
-    <hyperlink r:id="rId47" ref="E60"/>
-    <hyperlink r:id="rId48" ref="E62"/>
+    <hyperlink r:id="rId46" ref="E57"/>
+    <hyperlink r:id="rId47" ref="E59"/>
+    <hyperlink r:id="rId48" ref="E61"/>
     <hyperlink r:id="rId49" ref="E63"/>
     <hyperlink r:id="rId50" ref="E64"/>
     <hyperlink r:id="rId51" ref="E65"/>
     <hyperlink r:id="rId52" ref="E66"/>
-    <hyperlink r:id="rId53" ref="E68"/>
-    <hyperlink r:id="rId54" ref="E72"/>
-    <hyperlink r:id="rId55" ref="E74"/>
+    <hyperlink r:id="rId53" ref="E67"/>
+    <hyperlink r:id="rId54" ref="E69"/>
+    <hyperlink r:id="rId55" ref="E73"/>
     <hyperlink r:id="rId56" ref="E75"/>
-    <hyperlink r:id="rId57" ref="E78"/>
+    <hyperlink r:id="rId57" ref="E76"/>
     <hyperlink r:id="rId58" ref="E79"/>
     <hyperlink r:id="rId59" ref="E80"/>
     <hyperlink r:id="rId60" ref="E81"/>
     <hyperlink r:id="rId61" ref="E82"/>
-    <hyperlink r:id="rId61" ref="E83"/>
-    <hyperlink r:id="rId61" ref="E84"/>
+    <hyperlink r:id="rId62" ref="E83"/>
+    <hyperlink r:id="rId62" ref="E84"/>
     <hyperlink r:id="rId62" ref="E85"/>
     <hyperlink r:id="rId63" ref="E86"/>
     <hyperlink r:id="rId64" ref="E87"/>
+    <hyperlink r:id="rId65" ref="E88"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>